<commit_message>
eeej map complete and huge
</commit_message>
<xml_diff>
--- a/data/Regional Analysis/R2R Regions - Summary Table.xlsx
+++ b/data/Regional Analysis/R2R Regions - Summary Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong138\Documents\Postdoc Research\Getting to Neutral - USA\Regions\Summaries from other chapters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stanley27\Desktop\cdr_maps\data\Regional Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C959946-3D32-443C-9DC9-86E3301A2A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C1B184-D525-4A44-B08D-2169BE5A77DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31185" yWindow="7140" windowWidth="19755" windowHeight="12495" xr2:uid="{269894C5-E869-441E-B323-488539907077}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{269894C5-E869-441E-B323-488539907077}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabulated Data" sheetId="3" r:id="rId1"/>
@@ -470,6 +470,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -483,21 +498,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,7 +827,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,57 +848,57 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" s="22" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27" t="s">
+      <c r="L2" s="31"/>
+      <c r="M2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -2044,16 +2044,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2061,23 +2061,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="11a73144-f27d-4a0d-a19a-92caad943dfc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8A53973CCD7E4488E11924EB2254DF2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0278396fae167141979c9165b458ac2c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="11a73144-f27d-4a0d-a19a-92caad943dfc" xmlns:ns4="c7a287d5-b293-4594-ac78-d6922591b342" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8449876e72bfa1574efcf7fec6560bb7" ns3:_="" ns4:_="">
     <xsd:import namespace="11a73144-f27d-4a0d-a19a-92caad943dfc"/>
@@ -2298,32 +2281,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EABDC11-C621-4E17-BEA9-2A2B4F762869}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="11a73144-f27d-4a0d-a19a-92caad943dfc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c7a287d5-b293-4594-ac78-d6922591b342"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8236962B-7966-4C13-B164-54129EC97B81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="11a73144-f27d-4a0d-a19a-92caad943dfc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5496342E-8CD5-4C58-B305-D79225C74FA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2340,4 +2315,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8236962B-7966-4C13-B164-54129EC97B81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EABDC11-C621-4E17-BEA9-2A2B4F762869}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="11a73144-f27d-4a0d-a19a-92caad943dfc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c7a287d5-b293-4594-ac78-d6922591b342"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>